<commit_message>
filtro y otras cosas
cosas
extra
</commit_message>
<xml_diff>
--- a/PruebaSQL/reporte.xlsx
+++ b/PruebaSQL/reporte.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ernes\OneDrive\Documentos\NetBeansProjects\tecnishop\PruebaSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65650DC-9927-4714-8F2B-8C337B93D852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D5792A-9890-4C59-A955-40BBA73D9C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FCDCA76E-44D6-436D-A96C-26E2A768E835}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$L$70</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -632,6 +635,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -650,6 +671,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -668,65 +713,26 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -736,78 +742,75 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1237,10 +1240,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267469BD-314E-436E-8B21-8758217793CF}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:L4"/>
+    <sheetView tabSelected="1" zoomScale="18" zoomScaleNormal="18" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1253,36 +1259,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67"/>
-      <c r="B1" s="68"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="70" t="s">
+      <c r="A1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="74" t="s">
+      <c r="J1" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="75"/>
-      <c r="L1" s="76"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="69"/>
     </row>
     <row r="2" spans="1:12" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="48"/>
+      <c r="A2" s="43"/>
       <c r="B2" s="41"/>
       <c r="C2" s="42"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="79"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="72"/>
     </row>
     <row r="3" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48"/>
+      <c r="A3" s="43"/>
       <c r="B3" s="41"/>
       <c r="C3" s="42"/>
       <c r="D3" s="10" t="s">
@@ -1290,14 +1296,14 @@
       </c>
       <c r="E3" s="21"/>
       <c r="F3" s="22"/>
-      <c r="J3" s="80" t="s">
+      <c r="J3" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="82"/>
-      <c r="L3" s="83"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="57"/>
     </row>
     <row r="4" spans="1:12" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="48"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="41"/>
       <c r="C4" s="42"/>
       <c r="D4" s="10" t="s">
@@ -1305,16 +1311,16 @@
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="22"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="85"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="59"/>
     </row>
     <row r="5" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="61"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="62"/>
       <c r="D5" s="10" t="s">
         <v>26</v>
       </c>
@@ -1331,35 +1337,35 @@
       <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
       <c r="F7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
       <c r="I7" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
-      <c r="L7" s="64"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="46"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
       <c r="F8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="66"/>
-      <c r="H8" s="62"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="75"/>
       <c r="I8" s="25"/>
       <c r="L8" s="13"/>
     </row>
@@ -1368,122 +1374,122 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="56" t="s">
+      <c r="B10" s="79"/>
+      <c r="C10" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="55" t="s">
+      <c r="D10" s="81"/>
+      <c r="E10" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="55"/>
-      <c r="G10" s="56" t="s">
+      <c r="F10" s="79"/>
+      <c r="G10" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="57"/>
-      <c r="I10" s="55" t="s">
+      <c r="H10" s="81"/>
+      <c r="I10" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="58"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="82"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="48"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="41"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="50"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="44"/>
       <c r="E11" s="41"/>
       <c r="F11" s="41"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="53"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="84"/>
+      <c r="K11" s="84"/>
+      <c r="L11" s="85"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="48"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="41"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="50"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="44"/>
       <c r="E12" s="41"/>
       <c r="F12" s="41"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="49"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="40"/>
       <c r="J12" s="41"/>
       <c r="K12" s="41"/>
       <c r="L12" s="42"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="48"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="41"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="50"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="44"/>
       <c r="E13" s="41"/>
       <c r="F13" s="41"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="49"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="40"/>
       <c r="J13" s="41"/>
       <c r="K13" s="41"/>
       <c r="L13" s="42"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="48"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="41"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="50"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="44"/>
       <c r="E14" s="41"/>
       <c r="F14" s="41"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="49"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="40"/>
       <c r="J14" s="41"/>
       <c r="K14" s="41"/>
       <c r="L14" s="42"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="48"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="41"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="50"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="44"/>
       <c r="E15" s="41"/>
       <c r="F15" s="41"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="49"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="40"/>
       <c r="J15" s="41"/>
       <c r="K15" s="41"/>
       <c r="L15" s="42"/>
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="43"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="47"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="30"/>
     </row>
     <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="28"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -1496,8 +1502,8 @@
       <c r="L18" s="15"/>
     </row>
     <row r="19" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="29"/>
-      <c r="B19" s="30"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="36"/>
       <c r="D19" s="8" t="s">
         <v>7</v>
       </c>
@@ -1517,13 +1523,13 @@
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="29"/>
-      <c r="B20" s="30"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="36"/>
       <c r="L20" s="13"/>
     </row>
     <row r="21" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="29"/>
-      <c r="B21" s="30"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="36"/>
       <c r="D21" s="6" t="s">
         <v>3</v>
       </c>
@@ -1537,8 +1543,8 @@
       <c r="L21" s="13"/>
     </row>
     <row r="22" spans="1:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
-      <c r="B22" s="32"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="38"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1551,94 +1557,94 @@
       <c r="L22" s="16"/>
     </row>
     <row r="23" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="35"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="49"/>
     </row>
     <row r="24" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="36"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="38"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="52"/>
       <c r="M24" s="11"/>
     </row>
     <row r="25" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="36"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="38"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="52"/>
       <c r="M25" s="11"/>
     </row>
     <row r="26" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="36"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="38"/>
+      <c r="A26" s="50"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="51"/>
+      <c r="L26" s="52"/>
       <c r="M26" s="11"/>
     </row>
     <row r="27" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="36"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="38"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="52"/>
       <c r="M27" s="11"/>
     </row>
     <row r="28" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="36"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="38"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="52"/>
       <c r="M28" s="11"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -1660,16 +1666,16 @@
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="J33" s="40" t="s">
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="J33" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="K33" s="40"/>
+      <c r="K33" s="32"/>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -1704,36 +1710,36 @@
       <c r="L35" s="19"/>
     </row>
     <row r="36" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="67"/>
-      <c r="B36" s="68"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="70" t="s">
+      <c r="A36" s="53"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="71"/>
-      <c r="F36" s="71"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
-      <c r="J36" s="74" t="s">
+      <c r="J36" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="K36" s="75"/>
-      <c r="L36" s="76"/>
+      <c r="K36" s="68"/>
+      <c r="L36" s="69"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="48"/>
+      <c r="A37" s="43"/>
       <c r="B37" s="41"/>
       <c r="C37" s="42"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
-      <c r="J37" s="77"/>
-      <c r="K37" s="78"/>
-      <c r="L37" s="79"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="71"/>
+      <c r="L37" s="72"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="48"/>
+      <c r="A38" s="43"/>
       <c r="B38" s="41"/>
       <c r="C38" s="42"/>
       <c r="D38" s="10" t="s">
@@ -1741,14 +1747,14 @@
       </c>
       <c r="E38" s="21"/>
       <c r="F38" s="22"/>
-      <c r="J38" s="80" t="s">
+      <c r="J38" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="K38" s="82"/>
-      <c r="L38" s="83"/>
+      <c r="K38" s="56"/>
+      <c r="L38" s="57"/>
     </row>
     <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="48"/>
+      <c r="A39" s="43"/>
       <c r="B39" s="41"/>
       <c r="C39" s="42"/>
       <c r="D39" s="10" t="s">
@@ -1756,16 +1762,16 @@
       </c>
       <c r="E39" s="21"/>
       <c r="F39" s="22"/>
-      <c r="J39" s="81"/>
-      <c r="K39" s="84"/>
-      <c r="L39" s="85"/>
+      <c r="J39" s="74"/>
+      <c r="K39" s="58"/>
+      <c r="L39" s="59"/>
     </row>
     <row r="40" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A40" s="59" t="s">
+      <c r="A40" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="60"/>
-      <c r="C40" s="61"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="62"/>
       <c r="D40" s="10" t="s">
         <v>26</v>
       </c>
@@ -1782,35 +1788,35 @@
       <c r="A42" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="62"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
+      <c r="B42" s="75"/>
+      <c r="C42" s="75"/>
+      <c r="D42" s="75"/>
+      <c r="E42" s="75"/>
       <c r="F42" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G42" s="62"/>
-      <c r="H42" s="62"/>
+      <c r="G42" s="75"/>
+      <c r="H42" s="75"/>
       <c r="I42" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="J42" s="63"/>
-      <c r="K42" s="63"/>
-      <c r="L42" s="64"/>
+      <c r="J42" s="45"/>
+      <c r="K42" s="45"/>
+      <c r="L42" s="46"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="65"/>
-      <c r="C43" s="62"/>
-      <c r="D43" s="62"/>
-      <c r="E43" s="62"/>
+      <c r="B43" s="76"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="75"/>
       <c r="F43" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="66"/>
-      <c r="H43" s="62"/>
+      <c r="G43" s="77"/>
+      <c r="H43" s="75"/>
       <c r="I43" s="25"/>
       <c r="L43" s="13"/>
     </row>
@@ -1819,122 +1825,122 @@
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="54" t="s">
+      <c r="A45" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="55"/>
-      <c r="C45" s="56" t="s">
+      <c r="B45" s="79"/>
+      <c r="C45" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="D45" s="57"/>
-      <c r="E45" s="55" t="s">
+      <c r="D45" s="81"/>
+      <c r="E45" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="F45" s="55"/>
-      <c r="G45" s="56" t="s">
+      <c r="F45" s="79"/>
+      <c r="G45" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="H45" s="57"/>
-      <c r="I45" s="55" t="s">
+      <c r="H45" s="81"/>
+      <c r="I45" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="J45" s="55"/>
-      <c r="K45" s="55"/>
-      <c r="L45" s="58"/>
+      <c r="J45" s="79"/>
+      <c r="K45" s="79"/>
+      <c r="L45" s="82"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="48"/>
+      <c r="A46" s="43"/>
       <c r="B46" s="41"/>
-      <c r="C46" s="49"/>
-      <c r="D46" s="50"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="44"/>
       <c r="E46" s="41"/>
       <c r="F46" s="41"/>
-      <c r="G46" s="49"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="51"/>
-      <c r="J46" s="52"/>
-      <c r="K46" s="52"/>
-      <c r="L46" s="53"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="83"/>
+      <c r="J46" s="84"/>
+      <c r="K46" s="84"/>
+      <c r="L46" s="85"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="48"/>
+      <c r="A47" s="43"/>
       <c r="B47" s="41"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="50"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="44"/>
       <c r="E47" s="41"/>
       <c r="F47" s="41"/>
-      <c r="G47" s="49"/>
-      <c r="H47" s="50"/>
-      <c r="I47" s="49"/>
+      <c r="G47" s="40"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="40"/>
       <c r="J47" s="41"/>
       <c r="K47" s="41"/>
       <c r="L47" s="42"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="48"/>
+      <c r="A48" s="43"/>
       <c r="B48" s="41"/>
-      <c r="C48" s="49"/>
-      <c r="D48" s="50"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="44"/>
       <c r="E48" s="41"/>
       <c r="F48" s="41"/>
-      <c r="G48" s="49"/>
-      <c r="H48" s="50"/>
-      <c r="I48" s="49"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="40"/>
       <c r="J48" s="41"/>
       <c r="K48" s="41"/>
       <c r="L48" s="42"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="48"/>
+      <c r="A49" s="43"/>
       <c r="B49" s="41"/>
-      <c r="C49" s="49"/>
-      <c r="D49" s="50"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="44"/>
       <c r="E49" s="41"/>
       <c r="F49" s="41"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="50"/>
-      <c r="I49" s="49"/>
+      <c r="G49" s="40"/>
+      <c r="H49" s="44"/>
+      <c r="I49" s="40"/>
       <c r="J49" s="41"/>
       <c r="K49" s="41"/>
       <c r="L49" s="42"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50" s="48"/>
+      <c r="A50" s="43"/>
       <c r="B50" s="41"/>
-      <c r="C50" s="49"/>
-      <c r="D50" s="50"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="44"/>
       <c r="E50" s="41"/>
       <c r="F50" s="41"/>
-      <c r="G50" s="49"/>
-      <c r="H50" s="50"/>
-      <c r="I50" s="49"/>
+      <c r="G50" s="40"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="40"/>
       <c r="J50" s="41"/>
       <c r="K50" s="41"/>
       <c r="L50" s="42"/>
     </row>
     <row r="51" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="43"/>
-      <c r="B51" s="44"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="46"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="45"/>
-      <c r="H51" s="46"/>
-      <c r="I51" s="45"/>
-      <c r="J51" s="44"/>
-      <c r="K51" s="44"/>
-      <c r="L51" s="47"/>
+      <c r="A51" s="39"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="27"/>
+      <c r="J51" s="29"/>
+      <c r="K51" s="29"/>
+      <c r="L51" s="30"/>
     </row>
     <row r="52" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="14"/>
       <c r="L52" s="13"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="27" t="s">
+      <c r="A53" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="28"/>
+      <c r="B53" s="34"/>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
@@ -1947,8 +1953,8 @@
       <c r="L53" s="15"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="29"/>
-      <c r="B54" s="30"/>
+      <c r="A54" s="35"/>
+      <c r="B54" s="36"/>
       <c r="D54" s="8" t="s">
         <v>7</v>
       </c>
@@ -1968,13 +1974,13 @@
       <c r="L54" s="13"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55" s="29"/>
-      <c r="B55" s="30"/>
+      <c r="A55" s="35"/>
+      <c r="B55" s="36"/>
       <c r="L55" s="13"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56" s="29"/>
-      <c r="B56" s="30"/>
+      <c r="A56" s="35"/>
+      <c r="B56" s="36"/>
       <c r="D56" s="6" t="s">
         <v>3</v>
       </c>
@@ -1988,8 +1994,8 @@
       <c r="L56" s="13"/>
     </row>
     <row r="57" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="31"/>
-      <c r="B57" s="32"/>
+      <c r="A57" s="37"/>
+      <c r="B57" s="38"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -2002,90 +2008,90 @@
       <c r="L57" s="16"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A58" s="33" t="s">
+      <c r="A58" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="B58" s="34"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="34"/>
-      <c r="H58" s="34"/>
-      <c r="I58" s="34"/>
-      <c r="J58" s="34"/>
-      <c r="K58" s="34"/>
-      <c r="L58" s="35"/>
+      <c r="B58" s="48"/>
+      <c r="C58" s="48"/>
+      <c r="D58" s="48"/>
+      <c r="E58" s="48"/>
+      <c r="F58" s="48"/>
+      <c r="G58" s="48"/>
+      <c r="H58" s="48"/>
+      <c r="I58" s="48"/>
+      <c r="J58" s="48"/>
+      <c r="K58" s="48"/>
+      <c r="L58" s="49"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A59" s="36"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="37"/>
-      <c r="H59" s="37"/>
-      <c r="I59" s="37"/>
-      <c r="J59" s="37"/>
-      <c r="K59" s="37"/>
-      <c r="L59" s="38"/>
+      <c r="A59" s="50"/>
+      <c r="B59" s="51"/>
+      <c r="C59" s="51"/>
+      <c r="D59" s="51"/>
+      <c r="E59" s="51"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="51"/>
+      <c r="H59" s="51"/>
+      <c r="I59" s="51"/>
+      <c r="J59" s="51"/>
+      <c r="K59" s="51"/>
+      <c r="L59" s="52"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" s="36"/>
-      <c r="B60" s="37"/>
-      <c r="C60" s="37"/>
-      <c r="D60" s="37"/>
-      <c r="E60" s="37"/>
-      <c r="F60" s="37"/>
-      <c r="G60" s="37"/>
-      <c r="H60" s="37"/>
-      <c r="I60" s="37"/>
-      <c r="J60" s="37"/>
-      <c r="K60" s="37"/>
-      <c r="L60" s="38"/>
+      <c r="A60" s="50"/>
+      <c r="B60" s="51"/>
+      <c r="C60" s="51"/>
+      <c r="D60" s="51"/>
+      <c r="E60" s="51"/>
+      <c r="F60" s="51"/>
+      <c r="G60" s="51"/>
+      <c r="H60" s="51"/>
+      <c r="I60" s="51"/>
+      <c r="J60" s="51"/>
+      <c r="K60" s="51"/>
+      <c r="L60" s="52"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="36"/>
-      <c r="B61" s="37"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="37"/>
-      <c r="H61" s="37"/>
-      <c r="I61" s="37"/>
-      <c r="J61" s="37"/>
-      <c r="K61" s="37"/>
-      <c r="L61" s="38"/>
+      <c r="A61" s="50"/>
+      <c r="B61" s="51"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="51"/>
+      <c r="E61" s="51"/>
+      <c r="F61" s="51"/>
+      <c r="G61" s="51"/>
+      <c r="H61" s="51"/>
+      <c r="I61" s="51"/>
+      <c r="J61" s="51"/>
+      <c r="K61" s="51"/>
+      <c r="L61" s="52"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62" s="36"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="37"/>
-      <c r="H62" s="37"/>
-      <c r="I62" s="37"/>
-      <c r="J62" s="37"/>
-      <c r="K62" s="37"/>
-      <c r="L62" s="38"/>
+      <c r="A62" s="50"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="51"/>
+      <c r="E62" s="51"/>
+      <c r="F62" s="51"/>
+      <c r="G62" s="51"/>
+      <c r="H62" s="51"/>
+      <c r="I62" s="51"/>
+      <c r="J62" s="51"/>
+      <c r="K62" s="51"/>
+      <c r="L62" s="52"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" s="36"/>
-      <c r="B63" s="37"/>
-      <c r="C63" s="37"/>
-      <c r="D63" s="37"/>
-      <c r="E63" s="37"/>
-      <c r="F63" s="37"/>
-      <c r="G63" s="37"/>
-      <c r="H63" s="37"/>
-      <c r="I63" s="37"/>
-      <c r="J63" s="37"/>
-      <c r="K63" s="37"/>
-      <c r="L63" s="38"/>
+      <c r="A63" s="50"/>
+      <c r="B63" s="51"/>
+      <c r="C63" s="51"/>
+      <c r="D63" s="51"/>
+      <c r="E63" s="51"/>
+      <c r="F63" s="51"/>
+      <c r="G63" s="51"/>
+      <c r="H63" s="51"/>
+      <c r="I63" s="51"/>
+      <c r="J63" s="51"/>
+      <c r="K63" s="51"/>
+      <c r="L63" s="52"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="14"/>
@@ -2104,16 +2110,16 @@
       <c r="L67" s="13"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A68" s="39" t="s">
+      <c r="A68" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B68" s="40"/>
-      <c r="C68" s="40"/>
-      <c r="D68" s="40"/>
-      <c r="J68" s="40" t="s">
+      <c r="B68" s="32"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="32"/>
+      <c r="J68" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="K68" s="40"/>
+      <c r="K68" s="32"/>
       <c r="L68" s="13"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
@@ -2149,34 +2155,58 @@
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="A18:B22"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="A53:B57"/>
+    <mergeCell ref="A58:L63"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="J69:L69"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="I51:L51"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:L50"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:L49"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:L48"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I47:L47"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I46:L46"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:L45"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="A36:C39"/>
+    <mergeCell ref="D36:F37"/>
+    <mergeCell ref="J36:L37"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="K38:L39"/>
     <mergeCell ref="J34:L34"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="J7:L7"/>
@@ -2201,61 +2231,37 @@
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="I11:L11"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="A36:C39"/>
-    <mergeCell ref="D36:F37"/>
-    <mergeCell ref="J36:L37"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="K38:L39"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I46:L46"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:L45"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:L48"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="I47:L47"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:L50"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="I49:L49"/>
-    <mergeCell ref="A53:B57"/>
-    <mergeCell ref="A58:L63"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="J69:L69"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="I51:L51"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="A18:B22"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="64" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>